<commit_message>
Major update on all scripts
</commit_message>
<xml_diff>
--- a/outputs/reconciled_data_CPAxtra.xlsx
+++ b/outputs/reconciled_data_CPAxtra.xlsx
@@ -465,7 +465,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tax Branch</t>
+          <t>Tax Branch</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -587,7 +587,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -610,8 +610,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>127</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -670,7 +672,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -693,8 +695,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>127</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -751,7 +755,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="U3" t="n">
@@ -779,7 +783,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -802,8 +806,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>127</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -860,7 +866,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="U4" t="n">
@@ -888,7 +894,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -911,8 +917,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>127</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -969,7 +977,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="U5" t="n">
@@ -997,7 +1005,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1020,8 +1028,10 @@
           <t>สัตหีบ</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>150</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>00150</t>
+        </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -1078,7 +1088,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="U6" t="n">
@@ -1106,7 +1116,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1129,8 +1139,10 @@
           <t>สัตหีบ</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>150</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>00150</t>
+        </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1187,7 +1199,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="U7" t="n">
@@ -1215,7 +1227,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1238,8 +1250,10 @@
           <t>รามอินทรา</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>53</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>00053</t>
+        </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1248,7 +1262,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>5087</t>
+          <t>05087</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1296,7 +1310,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1319,8 +1333,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F9" t="n">
-        <v>58</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1377,7 +1393,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="U9" t="n">
@@ -1405,7 +1421,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1428,8 +1444,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>91</v>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1486,7 +1504,7 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="U10" t="n">
@@ -1514,7 +1532,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1537,8 +1555,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>127</v>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1547,7 +1567,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1595,7 +1615,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1618,8 +1638,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>127</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1676,7 +1698,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1699,8 +1721,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F13" t="n">
-        <v>127</v>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1759,7 +1783,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1782,8 +1806,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F14" t="n">
-        <v>127</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1840,7 +1866,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1863,8 +1889,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F15" t="n">
-        <v>151</v>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1873,7 +1901,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1921,7 +1949,7 @@
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="U15" t="n">
@@ -1949,7 +1977,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1972,8 +2000,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F16" t="n">
-        <v>151</v>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1982,7 +2012,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -2030,7 +2060,7 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="U16" t="n">
@@ -2058,7 +2088,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2081,8 +2111,10 @@
           <t>เชียงใหม่ 2</t>
         </is>
       </c>
-      <c r="F17" t="n">
-        <v>44</v>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>00044</t>
+        </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -2091,7 +2123,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>5011</t>
+          <t>05011</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -2139,7 +2171,7 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="U17" t="n">
@@ -2167,7 +2199,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2190,8 +2222,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F18" t="n">
-        <v>58</v>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -2248,7 +2282,7 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="U18" t="n">
@@ -2276,7 +2310,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2299,8 +2333,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F19" t="n">
-        <v>91</v>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -2357,7 +2393,7 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="U19" t="n">
@@ -2385,7 +2421,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2408,8 +2444,10 @@
           <t>สัตหีบ</t>
         </is>
       </c>
-      <c r="F20" t="n">
-        <v>150</v>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>00150</t>
+        </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -2466,7 +2504,7 @@
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U20" t="n">
@@ -2494,7 +2532,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2517,8 +2555,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F21" t="n">
-        <v>151</v>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -2527,7 +2567,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2575,7 +2615,7 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U21" t="n">
@@ -2605,7 +2645,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2628,8 +2668,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F22" t="n">
-        <v>151</v>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -2638,7 +2680,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -2686,7 +2728,7 @@
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U22" t="n">
@@ -2716,7 +2758,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2739,8 +2781,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F23" t="n">
-        <v>151</v>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -2749,7 +2793,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2797,7 +2841,7 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U23" t="n">
@@ -2827,7 +2871,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2850,8 +2894,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F24" t="n">
-        <v>58</v>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -2908,7 +2954,7 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U24" t="n">
@@ -2936,7 +2982,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2959,8 +3005,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F25" t="n">
-        <v>58</v>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -3017,7 +3065,7 @@
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U25" t="n">
@@ -3045,7 +3093,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3068,8 +3116,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F26" t="n">
-        <v>58</v>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -3126,7 +3176,7 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U26" t="n">
@@ -3156,7 +3206,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3179,8 +3229,10 @@
           <t>นครราชสีมา</t>
         </is>
       </c>
-      <c r="F27" t="n">
-        <v>7</v>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>00007</t>
+        </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -3189,7 +3241,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>5024</t>
+          <t>05024</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -3237,7 +3289,7 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U27" t="n">
@@ -3265,7 +3317,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3288,8 +3340,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F28" t="n">
-        <v>91</v>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -3346,7 +3400,7 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U28" t="n">
@@ -3374,7 +3428,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>04/11/2023</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3397,8 +3451,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F29" t="n">
-        <v>127</v>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -3407,7 +3463,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -3455,7 +3511,7 @@
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>04/11/2023</t>
         </is>
       </c>
       <c r="U29" t="n">
@@ -3483,7 +3539,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>04/11/2023</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3506,8 +3562,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F30" t="n">
-        <v>151</v>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -3516,7 +3574,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -3564,7 +3622,7 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>04/11/2023</t>
         </is>
       </c>
       <c r="U30" t="n">
@@ -3592,7 +3650,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>04/11/2023</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3615,8 +3673,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F31" t="n">
-        <v>151</v>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -3625,7 +3685,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -3673,7 +3733,7 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>04/11/2023</t>
         </is>
       </c>
       <c r="U31" t="n">
@@ -3701,7 +3761,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>05/11/2023</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3724,8 +3784,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F32" t="n">
-        <v>127</v>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -3734,7 +3796,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -3782,7 +3844,7 @@
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>05/11/2023</t>
         </is>
       </c>
       <c r="U32" t="n">
@@ -3810,7 +3872,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>05/11/2023</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3833,8 +3895,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F33" t="n">
-        <v>127</v>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -3843,7 +3907,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -3891,7 +3955,7 @@
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>05/11/2023</t>
         </is>
       </c>
       <c r="U33" t="n">
@@ -3919,7 +3983,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>05/11/2023</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3942,8 +4006,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F34" t="n">
-        <v>58</v>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -4000,7 +4066,7 @@
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>05/11/2023</t>
         </is>
       </c>
       <c r="U34" t="n">
@@ -4028,7 +4094,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4051,8 +4117,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F35" t="n">
-        <v>127</v>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -4061,7 +4129,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -4109,7 +4177,7 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U35" t="n">
@@ -4137,7 +4205,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4160,8 +4228,10 @@
           <t>สัตหีบ</t>
         </is>
       </c>
-      <c r="F36" t="n">
-        <v>150</v>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>00150</t>
+        </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -4218,7 +4288,7 @@
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U36" t="n">
@@ -4246,7 +4316,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4269,8 +4339,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F37" t="n">
-        <v>151</v>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -4279,7 +4351,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -4327,7 +4399,7 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U37" t="n">
@@ -4355,7 +4427,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4378,8 +4450,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F38" t="n">
-        <v>151</v>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -4388,7 +4462,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -4436,7 +4510,7 @@
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U38" t="n">
@@ -4464,7 +4538,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4487,8 +4561,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F39" t="n">
-        <v>151</v>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -4497,7 +4573,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -4545,7 +4621,7 @@
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U39" t="n">
@@ -4573,7 +4649,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4596,8 +4672,10 @@
           <t>เชียงใหม่ 2</t>
         </is>
       </c>
-      <c r="F40" t="n">
-        <v>44</v>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>00044</t>
+        </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -4606,7 +4684,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>5011</t>
+          <t>05011</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -4654,7 +4732,7 @@
       </c>
       <c r="T40" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U40" t="n">
@@ -4682,7 +4760,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4705,8 +4783,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F41" t="n">
-        <v>58</v>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4763,7 +4843,7 @@
       </c>
       <c r="T41" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U41" t="n">
@@ -4791,7 +4871,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4814,8 +4894,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F42" t="n">
-        <v>58</v>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -4872,7 +4954,7 @@
       </c>
       <c r="T42" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U42" t="n">
@@ -4902,7 +4984,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4925,8 +5007,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F43" t="n">
-        <v>58</v>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4983,7 +5067,7 @@
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U43" t="n">
@@ -5013,7 +5097,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5036,8 +5120,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F44" t="n">
-        <v>58</v>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -5094,7 +5180,7 @@
       </c>
       <c r="T44" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U44" t="n">
@@ -5124,7 +5210,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5147,8 +5233,10 @@
           <t>รังสิต</t>
         </is>
       </c>
-      <c r="F45" t="n">
-        <v>8</v>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>00008</t>
+        </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -5157,7 +5245,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>6650</t>
+          <t>06650</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -5205,7 +5293,7 @@
       </c>
       <c r="T45" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>06/11/2023</t>
         </is>
       </c>
       <c r="U45" t="n">
@@ -5235,7 +5323,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5258,8 +5346,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F46" t="n">
-        <v>58</v>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -5316,7 +5406,7 @@
       </c>
       <c r="T46" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="U46" t="n">
@@ -5344,7 +5434,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5367,8 +5457,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F47" t="n">
-        <v>58</v>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -5425,7 +5517,7 @@
       </c>
       <c r="T47" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="U47" t="n">
@@ -5453,7 +5545,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5476,8 +5568,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F48" t="n">
-        <v>58</v>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -5534,7 +5628,7 @@
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="U48" t="n">
@@ -5564,7 +5658,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5587,8 +5681,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F49" t="n">
-        <v>91</v>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -5645,7 +5741,7 @@
       </c>
       <c r="T49" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="U49" t="n">
@@ -5673,7 +5769,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5696,8 +5792,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F50" t="n">
-        <v>91</v>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -5754,7 +5852,7 @@
       </c>
       <c r="T50" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="U50" t="n">
@@ -5782,7 +5880,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5805,8 +5903,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F51" t="n">
-        <v>91</v>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -5863,7 +5963,7 @@
       </c>
       <c r="T51" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="U51" t="n">
@@ -5891,7 +5991,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>08/11/2023</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5914,8 +6014,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F52" t="n">
-        <v>127</v>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -5924,7 +6026,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -5972,7 +6074,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>08/11/2023</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5995,8 +6097,10 @@
           <t>สัตหีบ</t>
         </is>
       </c>
-      <c r="F53" t="n">
-        <v>150</v>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>00150</t>
+        </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -6053,7 +6157,7 @@
       </c>
       <c r="T53" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>08/11/2023</t>
         </is>
       </c>
       <c r="U53" t="n">
@@ -6081,7 +6185,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>08/11/2023</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -6104,8 +6208,10 @@
           <t>จรัญสนิทวงศ์</t>
         </is>
       </c>
-      <c r="F54" t="n">
-        <v>24</v>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>00024</t>
+        </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -6114,7 +6220,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>5048</t>
+          <t>05048</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -6162,7 +6268,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>08/11/2023</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -6185,8 +6291,10 @@
           <t>เชียงใหม่ 2</t>
         </is>
       </c>
-      <c r="F55" t="n">
-        <v>44</v>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>00044</t>
+        </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -6195,7 +6303,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>5011</t>
+          <t>05011</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -6243,7 +6351,7 @@
       </c>
       <c r="T55" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>08/11/2023</t>
         </is>
       </c>
       <c r="U55" t="n">
@@ -6271,7 +6379,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -6294,8 +6402,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F56" t="n">
-        <v>127</v>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -6304,7 +6414,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -6352,7 +6462,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -6375,8 +6485,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F57" t="n">
-        <v>127</v>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -6385,7 +6497,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -6435,7 +6547,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -6458,8 +6570,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F58" t="n">
-        <v>127</v>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -6468,7 +6582,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -6516,7 +6630,7 @@
       </c>
       <c r="T58" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="U58" t="n">
@@ -6544,7 +6658,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -6567,8 +6681,10 @@
           <t>สัตหีบ</t>
         </is>
       </c>
-      <c r="F59" t="n">
-        <v>150</v>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>00150</t>
+        </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -6625,7 +6741,7 @@
       </c>
       <c r="T59" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="U59" t="n">
@@ -6653,7 +6769,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -6676,8 +6792,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F60" t="n">
-        <v>58</v>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -6734,7 +6852,7 @@
       </c>
       <c r="T60" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="U60" t="n">
@@ -6762,7 +6880,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -6785,8 +6903,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F61" t="n">
-        <v>58</v>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -6843,7 +6963,7 @@
       </c>
       <c r="T61" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="U61" t="n">
@@ -6871,7 +6991,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -6894,8 +7014,10 @@
           <t>รังสิต</t>
         </is>
       </c>
-      <c r="F62" t="n">
-        <v>8</v>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>00008</t>
+        </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -6952,7 +7074,7 @@
       </c>
       <c r="T62" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="U62" t="n">
@@ -6980,7 +7102,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -7003,8 +7125,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F63" t="n">
-        <v>127</v>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -7013,7 +7137,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -7061,7 +7185,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -7084,8 +7208,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F64" t="n">
-        <v>127</v>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -7094,7 +7220,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -7142,7 +7268,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -7165,8 +7291,10 @@
           <t>สัตหีบ</t>
         </is>
       </c>
-      <c r="F65" t="n">
-        <v>150</v>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>00150</t>
+        </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -7223,7 +7351,7 @@
       </c>
       <c r="T65" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="U65" t="n">
@@ -7251,7 +7379,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -7274,8 +7402,10 @@
           <t>เชียงใหม่ 2</t>
         </is>
       </c>
-      <c r="F66" t="n">
-        <v>44</v>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>00044</t>
+        </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -7284,7 +7414,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>5011</t>
+          <t>05011</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -7332,7 +7462,7 @@
       </c>
       <c r="T66" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="U66" t="n">
@@ -7360,7 +7490,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -7383,8 +7513,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F67" t="n">
-        <v>58</v>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -7441,7 +7573,7 @@
       </c>
       <c r="T67" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="U67" t="n">
@@ -7469,7 +7601,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -7492,8 +7624,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F68" t="n">
-        <v>58</v>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -7550,7 +7684,7 @@
       </c>
       <c r="T68" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="U68" t="n">
@@ -7578,7 +7712,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>11/11/2023</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -7601,8 +7735,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F69" t="n">
-        <v>127</v>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -7611,7 +7747,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -7659,7 +7795,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>11/11/2023</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -7682,8 +7818,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F70" t="n">
-        <v>127</v>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -7692,7 +7830,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -7740,7 +7878,7 @@
       </c>
       <c r="T70" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>11/11/2023</t>
         </is>
       </c>
       <c r="U70" t="n">
@@ -7768,7 +7906,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>11/11/2023</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -7791,8 +7929,10 @@
           <t>เชียงใหม่ 2</t>
         </is>
       </c>
-      <c r="F71" t="n">
-        <v>44</v>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>00044</t>
+        </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -7801,7 +7941,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>5011</t>
+          <t>05011</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -7849,7 +7989,7 @@
       </c>
       <c r="T71" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>11/11/2023</t>
         </is>
       </c>
       <c r="U71" t="n">
@@ -7877,7 +8017,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>11/11/2023</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -7900,8 +8040,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F72" t="n">
-        <v>58</v>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -7958,7 +8100,7 @@
       </c>
       <c r="T72" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>11/11/2023</t>
         </is>
       </c>
       <c r="U72" t="n">
@@ -7986,7 +8128,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>12/11/2023</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -8009,8 +8151,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F73" t="n">
-        <v>127</v>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -8019,7 +8163,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -8067,7 +8211,7 @@
       </c>
       <c r="T73" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>12/11/2023</t>
         </is>
       </c>
       <c r="U73" t="n">
@@ -8095,7 +8239,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>12/11/2023</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -8118,8 +8262,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F74" t="n">
-        <v>127</v>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -8128,7 +8274,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -8176,7 +8322,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>12/11/2023</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -8199,8 +8345,10 @@
           <t>รามคำแหง 24</t>
         </is>
       </c>
-      <c r="F75" t="n">
-        <v>151</v>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>00151</t>
+        </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -8209,7 +8357,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>5112</t>
+          <t>05112</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -8257,7 +8405,7 @@
       </c>
       <c r="T75" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>12/11/2023</t>
         </is>
       </c>
       <c r="U75" t="n">
@@ -8285,7 +8433,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>12/11/2023</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -8308,8 +8456,10 @@
           <t>เชียงใหม่ 2</t>
         </is>
       </c>
-      <c r="F76" t="n">
-        <v>44</v>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>00044</t>
+        </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -8318,7 +8468,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>5011</t>
+          <t>05011</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -8366,7 +8516,7 @@
       </c>
       <c r="T76" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>12/11/2023</t>
         </is>
       </c>
       <c r="U76" t="n">
@@ -8394,7 +8544,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -8417,8 +8567,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F77" t="n">
-        <v>127</v>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -8427,7 +8579,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -8475,7 +8627,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -8498,8 +8650,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F78" t="n">
-        <v>127</v>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -8556,7 +8710,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -8579,8 +8733,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F79" t="n">
-        <v>127</v>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -8637,7 +8793,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -8660,8 +8816,10 @@
           <t>สัตหีบ</t>
         </is>
       </c>
-      <c r="F80" t="n">
-        <v>150</v>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>00150</t>
+        </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -8718,7 +8876,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -8741,8 +8899,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F81" t="n">
-        <v>58</v>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -8799,7 +8959,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -8822,8 +8982,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F82" t="n">
-        <v>58</v>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -8887,9 +9049,17 @@
       </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
-      <c r="F83" t="inlineStr"/>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>00nan</t>
+        </is>
+      </c>
       <c r="G83" t="inlineStr"/>
-      <c r="H83" t="inlineStr"/>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>00nan</t>
+        </is>
+      </c>
       <c r="I83" t="inlineStr"/>
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="n">
@@ -8968,7 +9138,7 @@
       </c>
       <c r="T84" t="inlineStr">
         <is>
-          <t>2023-10-31</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="U84" t="n">
@@ -9037,7 +9207,7 @@
       </c>
       <c r="T85" t="inlineStr">
         <is>
-          <t>2023-10-30</t>
+          <t>30/10/2023</t>
         </is>
       </c>
       <c r="U85" t="n">
@@ -9106,7 +9276,7 @@
       </c>
       <c r="T86" t="inlineStr">
         <is>
-          <t>2023-10-31</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="U86" t="n">
@@ -9175,7 +9345,7 @@
       </c>
       <c r="T87" t="inlineStr">
         <is>
-          <t>2023-10-31</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="U87" t="n">
@@ -9247,7 +9417,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tax Branch</t>
+          <t>Tax Branch</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -9364,7 +9534,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -9387,8 +9557,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>127</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -9445,7 +9617,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="U2" t="n">
@@ -9474,7 +9646,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -9497,8 +9669,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>91</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -9555,7 +9729,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="U3" t="n">
@@ -9584,7 +9758,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -9607,8 +9781,10 @@
           <t>นครราชสีมา</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>7</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>00007</t>
+        </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -9617,7 +9793,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>5024</t>
+          <t>05024</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -9665,7 +9841,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U4" t="n">
@@ -9694,7 +9870,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -9717,8 +9893,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>91</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -9775,7 +9953,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="U5" t="n">
@@ -9804,7 +9982,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>04/11/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -9827,8 +10005,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>127</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -9837,7 +10017,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -9885,7 +10065,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>04/11/2023</t>
         </is>
       </c>
       <c r="U6" t="n">
@@ -9914,7 +10094,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>05/11/2023</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -9937,8 +10117,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>127</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -9947,7 +10129,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -9995,7 +10177,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>05/11/2023</t>
         </is>
       </c>
       <c r="U7" t="n">
@@ -10024,7 +10206,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -10047,8 +10229,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>58</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -10105,7 +10289,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="U8" t="n">
@@ -10134,7 +10318,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -10157,8 +10341,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F9" t="n">
-        <v>91</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -10215,7 +10401,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="U9" t="n">
@@ -10244,7 +10430,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -10267,8 +10453,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>91</v>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -10325,7 +10513,7 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="U10" t="n">
@@ -10354,7 +10542,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -10377,8 +10565,10 @@
           <t>สมุทรสาคร</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>91</v>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>00091</t>
+        </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -10435,7 +10625,7 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>07/11/2023</t>
         </is>
       </c>
       <c r="U11" t="n">
@@ -10464,7 +10654,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -10487,8 +10677,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>127</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -10497,7 +10689,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -10545,7 +10737,7 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="U12" t="n">
@@ -10574,7 +10766,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>11/11/2023</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -10597,8 +10789,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F13" t="n">
-        <v>127</v>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -10607,7 +10801,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -10655,7 +10849,7 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>11/11/2023</t>
         </is>
       </c>
       <c r="U13" t="n">
@@ -10728,7 +10922,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tax Branch</t>
+          <t>Tax Branch</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -10891,7 +11085,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>2023-10-31</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="U2" t="n">
@@ -10960,7 +11154,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>2023-10-30</t>
+          <t>30/10/2023</t>
         </is>
       </c>
       <c r="U3" t="n">
@@ -11029,7 +11223,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>2023-10-31</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="U4" t="n">
@@ -11098,7 +11292,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>2023-10-31</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="U5" t="n">
@@ -11170,7 +11364,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tax Branch</t>
+          <t>Tax Branch</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -11292,7 +11486,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -11315,8 +11509,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>127</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -11375,7 +11571,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -11398,8 +11594,10 @@
           <t>รามอินทรา</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>53</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>00053</t>
+        </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -11408,7 +11606,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>5087</t>
+          <t>05087</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -11456,7 +11654,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -11479,8 +11677,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>127</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -11489,7 +11689,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -11537,7 +11737,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -11560,8 +11760,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>127</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -11618,7 +11820,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -11641,8 +11843,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>127</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -11701,7 +11905,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>02/11/2023</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -11724,8 +11928,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>127</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -11782,7 +11988,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>08/11/2023</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -11805,8 +12011,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>127</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -11815,7 +12023,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -11863,7 +12071,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>08/11/2023</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -11886,8 +12094,10 @@
           <t>จรัญสนิทวงศ์</t>
         </is>
       </c>
-      <c r="F9" t="n">
-        <v>24</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>00024</t>
+        </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -11896,7 +12106,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>5048</t>
+          <t>05048</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -11944,7 +12154,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -11967,8 +12177,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>127</v>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -11977,7 +12189,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -12025,7 +12237,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>09/11/2023</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -12048,8 +12260,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>127</v>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -12058,7 +12272,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -12108,7 +12322,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -12131,8 +12345,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>127</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -12141,7 +12357,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -12189,7 +12405,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>10/11/2023</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -12212,8 +12428,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F13" t="n">
-        <v>127</v>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -12222,7 +12440,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -12270,7 +12488,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>11/11/2023</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -12293,8 +12511,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F14" t="n">
-        <v>127</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -12303,7 +12523,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -12351,7 +12571,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>12/11/2023</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -12374,8 +12594,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F15" t="n">
-        <v>127</v>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -12384,7 +12606,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -12432,7 +12654,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -12455,8 +12677,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F16" t="n">
-        <v>127</v>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -12465,7 +12689,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>05073</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -12513,7 +12737,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -12536,8 +12760,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F17" t="n">
-        <v>127</v>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -12594,7 +12820,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -12617,8 +12843,10 @@
           <t>สิงห์บุรี</t>
         </is>
       </c>
-      <c r="F18" t="n">
-        <v>127</v>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>00127</t>
+        </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -12675,7 +12903,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -12698,8 +12926,10 @@
           <t>สัตหีบ</t>
         </is>
       </c>
-      <c r="F19" t="n">
-        <v>150</v>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>00150</t>
+        </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -12756,7 +12986,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -12779,8 +13009,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F20" t="n">
-        <v>58</v>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -12837,7 +13069,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -12860,8 +13092,10 @@
           <t>ลพบุรี</t>
         </is>
       </c>
-      <c r="F21" t="n">
-        <v>58</v>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>00058</t>
+        </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -12925,9 +13159,17 @@
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>00nan</t>
+        </is>
+      </c>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>00nan</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">

</xml_diff>